<commit_message>
remove extra split delimiter (||) in background trait column for GCST002887
</commit_message>
<xml_diff>
--- a/trait-representation-migration/study_background_traits-ALL.xlsx
+++ b/trait-representation-migration/study_background_traits-ALL.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twhetzel/git/gwas-curation-utils/trait-representation-migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3193CE0-419A-9343-A234-140515085520}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9BF14C6-1721-BB4B-BCBC-64742BEE6584}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="2280" windowWidth="26840" windowHeight="15940" xr2:uid="{3696613E-24C1-A642-9595-4DC140265F10}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="study_background_traits-ALL" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -13951,10 +13951,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -13968,7 +13975,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13978,6 +13985,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -13994,10 +14007,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14315,8 +14329,8 @@
   <dimension ref="A1:E1518"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B152" sqref="B152"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F183" sqref="F183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17237,20 +17251,20 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A183" t="s">
+      <c r="A183" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B183" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C183" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="D183" t="s">
+      <c r="D183" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="E183" t="s">
-        <v>645</v>
+      <c r="E183" s="3" t="s">
+        <v>960</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
remove extra split delimiter (||) in background trait column for GCST002891
</commit_message>
<xml_diff>
--- a/trait-representation-migration/study_background_traits-ALL.xlsx
+++ b/trait-representation-migration/study_background_traits-ALL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twhetzel/git/gwas-curation-utils/trait-representation-migration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9BF14C6-1721-BB4B-BCBC-64742BEE6584}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B11908C0-26D8-BE4F-B122-09770A2F2D3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2300" yWindow="2280" windowWidth="26840" windowHeight="15940" xr2:uid="{3696613E-24C1-A642-9595-4DC140265F10}"/>
   </bookViews>
@@ -14007,11 +14007,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14330,7 +14331,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F183" sqref="F183"/>
+      <selection pane="bottomLeft" activeCell="A184" sqref="A184:E184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17268,20 +17269,20 @@
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A184" t="s">
+      <c r="A184" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="4" t="s">
         <v>647</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C184" s="4" t="s">
         <v>648</v>
       </c>
-      <c r="D184" t="s">
+      <c r="D184" s="4" t="s">
         <v>649</v>
       </c>
-      <c r="E184" t="s">
-        <v>645</v>
+      <c r="E184" s="4" t="s">
+        <v>960</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>